<commit_message>
2nd commit. Lecture 16 Section 1
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phild\IdeaProjects\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE225D5-8254-442F-9C5A-16A2F7B5FA43}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F56464-EED2-4140-8D3C-2F04BFAC7FC3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9660" xr2:uid="{E6DB4FF7-5C58-4D28-83FB-F9E578F5D8E7}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>firstname</t>
   </si>
@@ -49,6 +50,30 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Raman Arora</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Ishita</t>
+  </si>
+  <si>
+    <t>Rohit</t>
+  </si>
+  <si>
+    <t>Sehgal</t>
   </si>
 </sst>
 </file>
@@ -84,8 +109,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF3B8AE-5F4C-418F-8A11-F8C2D5DFDB02}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,6 +492,82 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30304DD7-7D89-4C67-8514-FDD6E9DB7DD0}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
3rd commit. Lecture 18 4:53 (just before data provider mod)
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phild\IdeaProjects\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F56464-EED2-4140-8D3C-2F04BFAC7FC3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4154CA7B-123C-4BDA-ACEF-2D7B99074C22}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9660" xr2:uid="{E6DB4FF7-5C58-4D28-83FB-F9E578F5D8E7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9660" activeTab="1" xr2:uid="{E6DB4FF7-5C58-4D28-83FB-F9E578F5D8E7}"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>firstname</t>
   </si>
@@ -74,6 +75,30 @@
   </si>
   <si>
     <t>Sehgal</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>runmode</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -455,16 +480,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF3B8AE-5F4C-418F-8A11-F8C2D5DFDB02}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D0BB37-9DA2-44C4-BD2E-99D0AAF01C29}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF3B8AE-5F4C-418F-8A11-F8C2D5DFDB02}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,8 +550,11 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -491,8 +567,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -505,8 +584,11 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -519,8 +601,11 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -532,6 +617,9 @@
       </c>
       <c r="D5" t="s">
         <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -539,7 +627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30304DD7-7D89-4C67-8514-FDD6E9DB7DD0}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>

<commit_message>
5 commit end of project 1
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phild\IdeaProjects\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4154CA7B-123C-4BDA-ACEF-2D7B99074C22}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2C8E4E-E234-44B1-8BE8-A900D0813BAD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9660" activeTab="1" xr2:uid="{E6DB4FF7-5C58-4D28-83FB-F9E578F5D8E7}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>firstname</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>runmode</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -532,7 +529,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,7 +582,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>